<commit_message>
Updated testing paf files and Excel files along with the JUnit tests
</commit_message>
<xml_diff>
--- a/pace-base/test_files/2811-KatzExcelExport.xlsx
+++ b/pace-base/test_files/2811-KatzExcelExport.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="525" windowWidth="27735" windowHeight="11955" firstSheet="12" activeTab="12"/>
+    <workbookView xWindow="105" yWindow="4125" windowWidth="21030" windowHeight="5670" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ApplicationDef" sheetId="1" r:id="rId1"/>
@@ -29,13 +29,14 @@
     <sheet name="CustomFunctions" sheetId="19" r:id="rId20"/>
     <sheet name="MemberTags" sheetId="20" r:id="rId21"/>
     <sheet name="RoundingRules" sheetId="21" r:id="rId22"/>
+    <sheet name="UserMemberlists" sheetId="23" r:id="rId23"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2984" uniqueCount="952">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3062" uniqueCount="964">
   <si>
     <t>app id</t>
   </si>
@@ -39128,12 +39129,48 @@
   <si>
     <t>4bac9cf1-4265-42b7-9ae8-27d074f09a27</t>
   </si>
+  <si>
+    <t>User Member Alias</t>
+  </si>
+  <si>
+    <t>Dimension Name</t>
+  </si>
+  <si>
+    <t>Member List</t>
+  </si>
+  <si>
+    <t>MyMeasures</t>
+  </si>
+  <si>
+    <t>@DESC(SLS_DLR)</t>
+  </si>
+  <si>
+    <t>SLS_AUR</t>
+  </si>
+  <si>
+    <t>read only measures (pipe delimited)</t>
+  </si>
+  <si>
+    <t>yearOffset</t>
+  </si>
+  <si>
+    <t>GUID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Default Style?</t>
+  </si>
+  <si>
+    <t>Migration Print Style #1 - RENAME</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="44">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="45">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -39356,6 +39393,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -39377,7 +39420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -39466,17 +39509,27 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -39550,6 +39603,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -39584,6 +39638,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -39759,7 +39814,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -40095,7 +40150,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -41495,7 +41550,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -41567,7 +41622,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -42249,10 +42304,10 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D78" sqref="D78:AR82"/>
     </sheetView>
@@ -51571,7 +51626,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -52637,7 +52692,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -53362,7 +53417,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -57970,12 +58025,12 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -57986,21 +58041,22 @@
     <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="321.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="66" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="48.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" customWidth="1"/>
+    <col min="8" max="8" width="321.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="66" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="30">
+    <row r="1" spans="1:19" ht="30">
       <c r="A1" s="34" t="s">
         <v>350</v>
       </c>
@@ -58019,44 +58075,47 @@
       <c r="F1" s="34" t="s">
         <v>756</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="44" t="s">
+        <v>958</v>
+      </c>
+      <c r="H1" s="34" t="s">
         <v>757</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="I1" s="34" t="s">
         <v>758</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="J1" s="34" t="s">
         <v>759</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="K1" s="34" t="s">
         <v>760</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="L1" s="34" t="s">
         <v>761</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="M1" s="34" t="s">
         <v>762</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="N1" s="34" t="s">
         <v>763</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="O1" s="34" t="s">
         <v>764</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="P1" s="34" t="s">
         <v>765</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="Q1" s="34" t="s">
         <v>766</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="R1" s="34" t="s">
         <v>767</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="S1" s="34" t="s">
         <v>768</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:19">
       <c r="A2" t="str">
         <f>Roles!$A$2</f>
         <v>Cat Mgr Merch Profit</v>
@@ -58079,27 +58138,27 @@
         <f>RuleSet_FSProfit!$A$2</f>
         <v>FSProfit</v>
       </c>
-      <c r="G2" t="str">
+      <c r="H2" t="str">
         <f>DynamicMembers!$B$2 &amp; " | " &amp; DynamicMembers!$B$3 &amp; " | " &amp; DynamicMembers!$B$4 &amp; " | " &amp; DynamicMembers!$B$5 &amp; " | " &amp; Versions!$A$6 &amp; " | " &amp; Versions!$A$4 &amp; " | " &amp; Versions!$A$8 &amp; " | " &amp; Versions!$A$9 &amp; " | " &amp; Versions!$A$11 &amp; " | " &amp; Versions!$A$12 &amp; " | " &amp; Versions!$A$22 &amp; " | " &amp; Versions!$A$24 &amp; " | " &amp; Versions!$A$26 &amp; " | " &amp; Versions!$A$27 &amp; " | " &amp; Versions!$A$23 &amp; " | " &amp; Versions!$A$40</f>
         <v>@PLAN_VERSION | @PLAN_VERSION.v.LYR | @PLAN_VERSION.v.LYR% | @PLAN_VERSION.%.TOTAL.YEAR | CMSP | MWP | LYR | PYR | CMWP.v.CMSP | CMWP.v.MWP | LYR.v.PYR | LYR.v.PYR.BP | CMWP.v.CMSP% | CMWP.v.MWP% | LYR.v.PYR% | LYR.%.TOTAL.YEAR</v>
       </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" t="str">
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="str">
         <f>ViewGroups!$A$40</f>
         <v>Cat Mgr Views</v>
       </c>
-      <c r="K2" t="str">
+      <c r="L2" t="str">
         <f>CustomMenus!$A$2 &amp; " | " &amp; CustomMenus!$A$4 &amp; " | " &amp; CustomMenus!$A$10 &amp; " | " &amp; CustomMenus!$A$12</f>
         <v>mnuP_LYR2WP | mnuP_CMWP2S | mnuP_MWP2CM | mnuP_MP2CM</v>
       </c>
-      <c r="L2" t="str">
+      <c r="M2" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:19">
       <c r="A3" t="str">
         <f>Roles!$A$3</f>
         <v>Cat Mgr Merch Profit Fcst</v>
@@ -58122,27 +58181,27 @@
         <f>RuleSet_FSProfit!$A$2</f>
         <v>FSProfit</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" t="str">
         <f>DynamicMembers!$B$2 &amp; " | " &amp; DynamicMembers!$B$3 &amp; " | " &amp; DynamicMembers!$B$4 &amp; " | " &amp; DynamicMembers!$B$5 &amp; " | " &amp; DynamicMembers!$B$6 &amp; " | " &amp; DynamicMembers!$B$7 &amp; " | " &amp; Versions!$A$7 &amp; " | " &amp; Versions!$A$47 &amp; " | " &amp; Versions!$A$45 &amp; " | " &amp; Versions!$A$8 &amp; " | " &amp; Versions!$A$9 &amp; " | " &amp; Versions!$A$50 &amp; " | " &amp; Versions!$A$51 &amp; " | " &amp; Versions!$A$22 &amp; " | " &amp; Versions!$A$65 &amp; " | " &amp; Versions!$A$66 &amp; " | " &amp; Versions!$A$23 &amp; " | " &amp; Versions!$A$40 &amp; " | " &amp; Versions!$A$41 &amp; " | " &amp; Versions!$A$79</f>
         <v>@PLAN_VERSION | @PLAN_VERSION.v.LYR | @PLAN_VERSION.v.LYR% | @PLAN_VERSION.%.TOTAL.YEAR | @PLAN_VERSION.v.MFP | @PLAN_VERSION.v.MFP% | MFP | CMSF | MWF | LYR | PYR | CMWF.v.CMSF | CMWF.v.MWF | LYR.v.PYR | CMWF.v.CMSF% | CMWF.v.MWF% | LYR.v.PYR% | LYR.%.TOTAL.YEAR | MFP.%.TOTAL.YEAR | MWF.%.TOTAL.YEAR</v>
       </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" t="str">
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="str">
         <f>ViewGroups!$A$2</f>
         <v>Fcst Cat Mgr Views</v>
       </c>
-      <c r="K3" t="str">
+      <c r="L3" t="str">
         <f>CustomMenus!$A$18 &amp; " | " &amp; CustomMenus!$A$24 &amp; " | " &amp; CustomMenus!$A$26</f>
         <v>mnuP_CMWF2S | mnuP_MWF2CM | mnuP_MF2CM</v>
       </c>
-      <c r="L3" t="str">
+      <c r="M3" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:19">
       <c r="A4" t="str">
         <f>Roles!$A$4</f>
         <v>Consolidated Merch Profit</v>
@@ -58165,19 +58224,19 @@
         <f>RuleSet_FSProfit!$A$2</f>
         <v>FSProfit</v>
       </c>
-      <c r="G4" t="str">
+      <c r="H4" t="str">
         <f>DynamicMembers!$B$2 &amp; " | " &amp; DynamicMembers!$B$3 &amp; " | " &amp; DynamicMembers!$B$4 &amp; " | " &amp; DynamicMembers!$B$5 &amp; " | " &amp; Versions!$A$4 &amp; " | " &amp; Versions!$A$8 &amp; " | " &amp; Versions!$A$9 &amp; " | " &amp; Versions!$A$21 &amp; " | " &amp; Versions!$A$22 &amp; " | " &amp; Versions!$A$36 &amp; " | " &amp; Versions!$A$23 &amp; " | " &amp; Versions!$A$38 &amp; " | " &amp; Versions!$A$40</f>
         <v>@PLAN_VERSION | @PLAN_VERSION.v.LYR | @PLAN_VERSION.v.LYR% | @PLAN_VERSION.%.TOTAL.YEAR | MWP | LYR | PYR | MP.v.MWP | LYR.v.PYR | MP.v.MWP% | LYR.v.PYR% | MWP.%.TOTAL.YEAR | LYR.%.TOTAL.YEAR</v>
       </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" t="str">
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="str">
         <f>ViewGroups!$A$54</f>
         <v>Merch Profit Views</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:19">
       <c r="A5" t="str">
         <f>Roles!$A$4</f>
         <v>Consolidated Merch Profit</v>
@@ -58200,19 +58259,19 @@
         <f>RuleSet_FSProfit!$A$2</f>
         <v>FSProfit</v>
       </c>
-      <c r="G5" t="str">
+      <c r="H5" t="str">
         <f>DynamicMembers!$B$2 &amp; " | " &amp; DynamicMembers!$B$3 &amp; " | " &amp; DynamicMembers!$B$4 &amp; " | " &amp; Versions!$A$6 &amp; " | " &amp; Versions!$A$5 &amp; " | " &amp; Versions!$A$8 &amp; " | " &amp; Versions!$A$9 &amp; " | " &amp; Versions!$A$16 &amp; " | " &amp; Versions!$A$17 &amp; " | " &amp; Versions!$A$22 &amp; " | " &amp; Versions!$A$31 &amp; " | " &amp; Versions!$A$32 &amp; " | " &amp; Versions!$A$23 &amp; " | " &amp; Versions!$A$39 &amp; " | " &amp; Versions!$A$40</f>
         <v>@PLAN_VERSION | @PLAN_VERSION.v.LYR | @PLAN_VERSION.v.LYR% | CMSP | MP | LYR | PYR | MWP.v.CMSP | MWP.v.MP | LYR.v.PYR | MWP.v.CMSP% | MWP.v.MP% | LYR.v.PYR% | MP.%.TOTAL.YEAR | LYR.%.TOTAL.YEAR</v>
       </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" t="str">
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" t="str">
         <f>ViewGroups!$A$54</f>
         <v>Merch Profit Views</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:19">
       <c r="A6" t="str">
         <f>Roles!$A$6</f>
         <v>Consolidated Merch Profit by CM</v>
@@ -58235,19 +58294,19 @@
         <f>RuleSet_FSProfit!$A$2</f>
         <v>FSProfit</v>
       </c>
-      <c r="G6" t="str">
+      <c r="H6" t="str">
         <f>DynamicMembers!$B$2 &amp; " | " &amp; DynamicMembers!$B$3 &amp; " | " &amp; DynamicMembers!$B$4 &amp; " | " &amp; Versions!$A$4 &amp; " | " &amp; Versions!$A$8 &amp; " | " &amp; Versions!$A$9 &amp; " | " &amp; Versions!$A$21 &amp; " | " &amp; Versions!$A$22 &amp; " | " &amp; Versions!$A$36 &amp; " | " &amp; Versions!$A$23 &amp; " | " &amp; Versions!$A$39 &amp; " | " &amp; Versions!$A$40</f>
         <v>@PLAN_VERSION | @PLAN_VERSION.v.LYR | @PLAN_VERSION.v.LYR% | MWP | LYR | PYR | MP.v.MWP | LYR.v.PYR | MP.v.MWP% | LYR.v.PYR% | MP.%.TOTAL.YEAR | LYR.%.TOTAL.YEAR</v>
       </c>
-      <c r="H6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" t="str">
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="str">
         <f>ViewGroups!$A$54</f>
         <v>Merch Profit Views</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:19">
       <c r="A7" t="str">
         <f>Roles!$A$6</f>
         <v>Consolidated Merch Profit by CM</v>
@@ -58270,19 +58329,19 @@
         <f>RuleSet_FSProfit!$A$2</f>
         <v>FSProfit</v>
       </c>
-      <c r="G7" t="str">
+      <c r="H7" t="str">
         <f>DynamicMembers!$B$2 &amp; " | " &amp; DynamicMembers!$B$3 &amp; " | " &amp; DynamicMembers!$B$4 &amp; " | " &amp; Versions!$A$6 &amp; " | " &amp; Versions!$A$5 &amp; " | " &amp; Versions!$A$8 &amp; " | " &amp; Versions!$A$9 &amp; " | " &amp; Versions!$A$16 &amp; " | " &amp; Versions!$A$17 &amp; " | " &amp; Versions!$A$22 &amp; " | " &amp; Versions!$A$31 &amp; " | " &amp; Versions!$A$32 &amp; " | " &amp; Versions!$A$23 &amp; " | " &amp; Versions!$A$40</f>
         <v>@PLAN_VERSION | @PLAN_VERSION.v.LYR | @PLAN_VERSION.v.LYR% | CMSP | MP | LYR | PYR | MWP.v.CMSP | MWP.v.MP | LYR.v.PYR | MWP.v.CMSP% | MWP.v.MP% | LYR.v.PYR% | LYR.%.TOTAL.YEAR</v>
       </c>
-      <c r="H7" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" t="str">
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" t="str">
         <f>ViewGroups!$A$54</f>
         <v>Merch Profit Views</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:19">
       <c r="A8" t="str">
         <f>Roles!$A$8</f>
         <v>LYR Update</v>
@@ -58305,27 +58364,27 @@
         <f>RuleSet_FSProfit!$A$2</f>
         <v>FSProfit</v>
       </c>
-      <c r="G8" t="str">
+      <c r="H8" t="str">
         <f>DynamicMembers!$B$2 &amp; " | " &amp; Versions!$A$9 &amp; " | " &amp; Versions!$A$22 &amp; " | " &amp; Versions!$A$23 &amp; " | " &amp; Versions!$A$40</f>
         <v>@PLAN_VERSION | PYR | LYR.v.PYR | LYR.v.PYR% | LYR.%.TOTAL.YEAR</v>
       </c>
-      <c r="H8" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" t="str">
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" t="str">
         <f>ViewGroups!$A$90</f>
         <v>LYR Update Views</v>
       </c>
-      <c r="K8" t="str">
+      <c r="L8" t="str">
         <f>CustomMenus!$A$14 &amp; " | " &amp; CustomMenus!$A$16</f>
         <v>mnuP_LYR2P | mnuP_LYR2PE</v>
       </c>
-      <c r="L8" t="str">
+      <c r="M8" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:19">
       <c r="A9" t="str">
         <f>Roles!$A$9</f>
         <v>LYR Update by CM</v>
@@ -58348,27 +58407,27 @@
         <f>RuleSet_FSProfit!$A$2</f>
         <v>FSProfit</v>
       </c>
-      <c r="G9" t="str">
+      <c r="H9" t="str">
         <f>DynamicMembers!$B$2 &amp; " | " &amp; Versions!$A$9 &amp; " | " &amp; Versions!$A$22 &amp; " | " &amp; Versions!$A$23 &amp; " | " &amp; Versions!$A$40</f>
         <v>@PLAN_VERSION | PYR | LYR.v.PYR | LYR.v.PYR% | LYR.%.TOTAL.YEAR</v>
       </c>
-      <c r="H9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9" t="str">
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" t="str">
         <f>ViewGroups!$A$90</f>
         <v>LYR Update Views</v>
       </c>
-      <c r="K9" t="str">
+      <c r="L9" t="str">
         <f>CustomMenus!$A$14 &amp; " | " &amp; CustomMenus!$A$16</f>
         <v>mnuP_LYR2P | mnuP_LYR2PE</v>
       </c>
-      <c r="L9" t="str">
+      <c r="M9" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:19">
       <c r="A10" t="str">
         <f>Roles!$A$10</f>
         <v>Merch Profit - COM Stores</v>
@@ -58391,27 +58450,27 @@
         <f>RuleSet_FSProfit!$A$2</f>
         <v>FSProfit</v>
       </c>
-      <c r="G10" t="str">
+      <c r="H10" t="str">
         <f>DynamicMembers!$B$2 &amp; " | " &amp; DynamicMembers!$B$3 &amp; " | " &amp; DynamicMembers!$B$4 &amp; " | " &amp; DynamicMembers!$B$5 &amp; " | " &amp; Versions!$A$4 &amp; " | " &amp; Versions!$A$8 &amp; " | " &amp; Versions!$A$9 &amp; " | " &amp; Versions!$A$21 &amp; " | " &amp; Versions!$A$22 &amp; " | " &amp; Versions!$A$24 &amp; " | " &amp; Versions!$A$36 &amp; " | " &amp; Versions!$A$23 &amp; " | " &amp; Versions!$A$38 &amp; " | " &amp; Versions!$A$40</f>
         <v>@PLAN_VERSION | @PLAN_VERSION.v.LYR | @PLAN_VERSION.v.LYR% | @PLAN_VERSION.%.TOTAL.YEAR | MWP | LYR | PYR | MP.v.MWP | LYR.v.PYR | LYR.v.PYR.BP | MP.v.MWP% | LYR.v.PYR% | MWP.%.TOTAL.YEAR | LYR.%.TOTAL.YEAR</v>
       </c>
-      <c r="H10" t="b">
-        <v>1</v>
-      </c>
-      <c r="J10" t="str">
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="str">
         <f>ViewGroups!$A$54</f>
         <v>Merch Profit Views</v>
       </c>
-      <c r="K10" t="str">
+      <c r="L10" t="str">
         <f>CustomMenus!$A$2 &amp; " | " &amp; CustomMenus!$A$8 &amp; " | " &amp; CustomMenus!$A$12</f>
         <v>mnuP_LYR2WP | mnuP_MWP2MP | mnuP_MP2CM</v>
       </c>
-      <c r="L10" t="str">
+      <c r="M10" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:19">
       <c r="A11" t="str">
         <f>Roles!$A$10</f>
         <v>Merch Profit - COM Stores</v>
@@ -58434,27 +58493,27 @@
         <f>RuleSet_FSProfit!$A$2</f>
         <v>FSProfit</v>
       </c>
-      <c r="G11" t="str">
+      <c r="H11" t="str">
         <f>DynamicMembers!$B$2 &amp; " | " &amp; DynamicMembers!$B$3 &amp; " | " &amp; DynamicMembers!$B$4 &amp; " | " &amp; DynamicMembers!$B$5 &amp; " | " &amp; Versions!$A$6 &amp; " | " &amp; Versions!$A$5 &amp; " | " &amp; Versions!$A$8 &amp; " | " &amp; Versions!$A$9 &amp; " | " &amp; Versions!$A$16 &amp; " | " &amp; Versions!$A$17 &amp; " | " &amp; Versions!$A$22 &amp; " | " &amp; Versions!$A$24 &amp; " | " &amp; Versions!$A$31 &amp; " | " &amp; Versions!$A$32 &amp; " | " &amp; Versions!$A$23 &amp; " | " &amp; Versions!$A$39 &amp; " | " &amp; Versions!$A$40</f>
         <v>@PLAN_VERSION | @PLAN_VERSION.v.LYR | @PLAN_VERSION.v.LYR% | @PLAN_VERSION.%.TOTAL.YEAR | CMSP | MP | LYR | PYR | MWP.v.CMSP | MWP.v.MP | LYR.v.PYR | LYR.v.PYR.BP | MWP.v.CMSP% | MWP.v.MP% | LYR.v.PYR% | MP.%.TOTAL.YEAR | LYR.%.TOTAL.YEAR</v>
       </c>
-      <c r="H11" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" t="str">
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" t="str">
         <f>ViewGroups!$A$54</f>
         <v>Merch Profit Views</v>
       </c>
-      <c r="K11" t="str">
+      <c r="L11" t="str">
         <f>CustomMenus!$A$2 &amp; " | " &amp; CustomMenus!$A$6 &amp; " | " &amp; CustomMenus!$A$8 &amp; " | " &amp; CustomMenus!$A$10</f>
         <v>mnuP_LYR2WP | mnuP_CSP2MW | mnuP_MWP2MP | mnuP_MWP2CM</v>
       </c>
-      <c r="L11" t="str">
+      <c r="M11" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:19">
       <c r="A12" t="str">
         <f>Roles!$A$12</f>
         <v>Merch Profit - Not COM Stores</v>
@@ -58477,27 +58536,27 @@
         <f>RuleSet_FSProfit!$A$2</f>
         <v>FSProfit</v>
       </c>
-      <c r="G12" t="str">
+      <c r="H12" t="str">
         <f>DynamicMembers!$B$2 &amp; " | " &amp; Versions!$A$4 &amp; " | " &amp; Versions!$A$21 &amp; " | " &amp; Versions!$A$36 &amp; " | " &amp; Versions!$A$43</f>
         <v>@PLAN_VERSION | MWP | MP.v.MWP | MP.v.MWP% | MP.%.TOT.FS.SALES</v>
       </c>
-      <c r="H12" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" t="str">
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="str">
         <f>ViewGroups!$A$108</f>
         <v>Not-Comp Views</v>
       </c>
-      <c r="K12" t="str">
+      <c r="L12" t="str">
         <f>CustomMenus!$A$8</f>
         <v>mnuP_MWP2MP</v>
       </c>
-      <c r="L12" t="str">
+      <c r="M12" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:19">
       <c r="A13" t="str">
         <f>Roles!$A$12</f>
         <v>Merch Profit - Not COM Stores</v>
@@ -58520,27 +58579,27 @@
         <f>RuleSet_FSProfit!$A$2</f>
         <v>FSProfit</v>
       </c>
-      <c r="G13" t="str">
+      <c r="H13" t="str">
         <f>DynamicMembers!$B$2 &amp; " | " &amp; Versions!$A$5 &amp; " | " &amp; Versions!$A$17 &amp; " | " &amp; Versions!$A$32 &amp; " | " &amp; Versions!$A$42</f>
         <v>@PLAN_VERSION | MP | MWP.v.MP | MWP.v.MP% | MWP.%.TOT.FS.SALES</v>
       </c>
-      <c r="H13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" t="str">
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" t="str">
         <f>ViewGroups!$A$108</f>
         <v>Not-Comp Views</v>
       </c>
-      <c r="K13" t="str">
+      <c r="L13" t="str">
         <f>CustomMenus!$A$8</f>
         <v>mnuP_MWP2MP</v>
       </c>
-      <c r="L13" t="str">
+      <c r="M13" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:19">
       <c r="A14" t="str">
         <f>Roles!$A$14</f>
         <v>Merch Profit by CM - COM Stores</v>
@@ -58563,27 +58622,27 @@
         <f>RuleSet_FSProfit!$A$2</f>
         <v>FSProfit</v>
       </c>
-      <c r="G14" t="str">
+      <c r="H14" t="str">
         <f>DynamicMembers!$B$2 &amp; " | " &amp; DynamicMembers!$B$3 &amp; " | " &amp; DynamicMembers!$B$4 &amp; " | " &amp; DynamicMembers!$B$5 &amp; " | " &amp; Versions!$A$4 &amp; " | " &amp; Versions!$A$8 &amp; " | " &amp; Versions!$A$9 &amp; " | " &amp; Versions!$A$21 &amp; " | " &amp; Versions!$A$22 &amp; " | " &amp; Versions!$A$24 &amp; " | " &amp; Versions!$A$36 &amp; " | " &amp; Versions!$A$23 &amp; " | " &amp; Versions!$A$38 &amp; " | " &amp; Versions!$A$40</f>
         <v>@PLAN_VERSION | @PLAN_VERSION.v.LYR | @PLAN_VERSION.v.LYR% | @PLAN_VERSION.%.TOTAL.YEAR | MWP | LYR | PYR | MP.v.MWP | LYR.v.PYR | LYR.v.PYR.BP | MP.v.MWP% | LYR.v.PYR% | MWP.%.TOTAL.YEAR | LYR.%.TOTAL.YEAR</v>
       </c>
-      <c r="H14" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" t="str">
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" t="str">
         <f>ViewGroups!$A$54</f>
         <v>Merch Profit Views</v>
       </c>
-      <c r="K14" t="str">
+      <c r="L14" t="str">
         <f>CustomMenus!$A$2 &amp; " | " &amp; CustomMenus!$A$8 &amp; " | " &amp; CustomMenus!$A$12</f>
         <v>mnuP_LYR2WP | mnuP_MWP2MP | mnuP_MP2CM</v>
       </c>
-      <c r="L14" t="str">
+      <c r="M14" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:19">
       <c r="A15" t="str">
         <f>Roles!$A$14</f>
         <v>Merch Profit by CM - COM Stores</v>
@@ -58606,27 +58665,27 @@
         <f>RuleSet_FSProfit!$A$2</f>
         <v>FSProfit</v>
       </c>
-      <c r="G15" t="str">
+      <c r="H15" t="str">
         <f>DynamicMembers!$B$2 &amp; " | " &amp; DynamicMembers!$B$3 &amp; " | " &amp; DynamicMembers!$B$4 &amp; " | " &amp; DynamicMembers!$B$5 &amp; " | " &amp; Versions!$A$6 &amp; " | " &amp; Versions!$A$5 &amp; " | " &amp; Versions!$A$8 &amp; " | " &amp; Versions!$A$9 &amp; " | " &amp; Versions!$A$16 &amp; " | " &amp; Versions!$A$17 &amp; " | " &amp; Versions!$A$22 &amp; " | " &amp; Versions!$A$24 &amp; " | " &amp; Versions!$A$31 &amp; " | " &amp; Versions!$A$32 &amp; " | " &amp; Versions!$A$23 &amp; " | " &amp; Versions!$A$39 &amp; " | " &amp; Versions!$A$40</f>
         <v>@PLAN_VERSION | @PLAN_VERSION.v.LYR | @PLAN_VERSION.v.LYR% | @PLAN_VERSION.%.TOTAL.YEAR | CMSP | MP | LYR | PYR | MWP.v.CMSP | MWP.v.MP | LYR.v.PYR | LYR.v.PYR.BP | MWP.v.CMSP% | MWP.v.MP% | LYR.v.PYR% | MP.%.TOTAL.YEAR | LYR.%.TOTAL.YEAR</v>
       </c>
-      <c r="H15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J15" t="str">
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" t="str">
         <f>ViewGroups!$A$54</f>
         <v>Merch Profit Views</v>
       </c>
-      <c r="K15" t="str">
+      <c r="L15" t="str">
         <f>CustomMenus!$A$2 &amp; " | " &amp; CustomMenus!$A$6 &amp; " | " &amp; CustomMenus!$A$8 &amp; " | " &amp; CustomMenus!$A$10</f>
         <v>mnuP_LYR2WP | mnuP_CSP2MW | mnuP_MWP2MP | mnuP_MWP2CM</v>
       </c>
-      <c r="L15" t="str">
+      <c r="M15" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:19">
       <c r="A16" t="str">
         <f>Roles!$A$16</f>
         <v>Merch Profit by CM - Not COM Stores</v>
@@ -58649,27 +58708,27 @@
         <f>RuleSet_FSProfit!$A$2</f>
         <v>FSProfit</v>
       </c>
-      <c r="G16" t="str">
+      <c r="H16" t="str">
         <f>DynamicMembers!$B$2 &amp; " | " &amp; Versions!$A$4 &amp; " | " &amp; Versions!$A$21 &amp; " | " &amp; Versions!$A$36 &amp; " | " &amp; Versions!$A$43</f>
         <v>@PLAN_VERSION | MWP | MP.v.MWP | MP.v.MWP% | MP.%.TOT.FS.SALES</v>
       </c>
-      <c r="H16" t="b">
-        <v>1</v>
-      </c>
-      <c r="J16" t="str">
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" t="str">
         <f>ViewGroups!$A$108</f>
         <v>Not-Comp Views</v>
       </c>
-      <c r="K16" t="str">
+      <c r="L16" t="str">
         <f>CustomMenus!$A$8</f>
         <v>mnuP_MWP2MP</v>
       </c>
-      <c r="L16" t="str">
+      <c r="M16" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:13">
       <c r="A17" t="str">
         <f>Roles!$A$16</f>
         <v>Merch Profit by CM - Not COM Stores</v>
@@ -58692,27 +58751,27 @@
         <f>RuleSet_FSProfit!$A$2</f>
         <v>FSProfit</v>
       </c>
-      <c r="G17" t="str">
+      <c r="H17" t="str">
         <f>DynamicMembers!$B$2 &amp; " | " &amp; Versions!$A$5 &amp; " | " &amp; Versions!$A$17 &amp; " | " &amp; Versions!$A$32 &amp; " | " &amp; Versions!$A$42</f>
         <v>@PLAN_VERSION | MP | MWP.v.MP | MWP.v.MP% | MWP.%.TOT.FS.SALES</v>
       </c>
-      <c r="H17" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" t="str">
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" t="str">
         <f>ViewGroups!$A$108</f>
         <v>Not-Comp Views</v>
       </c>
-      <c r="K17" t="str">
+      <c r="L17" t="str">
         <f>CustomMenus!$A$8</f>
         <v>mnuP_MWP2MP</v>
       </c>
-      <c r="L17" t="str">
+      <c r="M17" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:13">
       <c r="A18" t="str">
         <f>Roles!$A$18</f>
         <v>Merch Profit Fcst</v>
@@ -58735,27 +58794,27 @@
         <f>RuleSet_FSProfit!$A$2</f>
         <v>FSProfit</v>
       </c>
-      <c r="G18" t="str">
+      <c r="H18" t="str">
         <f>DynamicMembers!$B$2 &amp; " | " &amp; DynamicMembers!$B$3 &amp; " | " &amp; DynamicMembers!$B$4 &amp; " | " &amp; DynamicMembers!$B$5 &amp; " | " &amp; DynamicMembers!$B$6 &amp; " | " &amp; DynamicMembers!$B$7 &amp; " | " &amp; Versions!$A$7 &amp; " | " &amp; Versions!$A$45 &amp; " | " &amp; Versions!$A$8 &amp; " | " &amp; Versions!$A$9 &amp; " | " &amp; Versions!$A$62 &amp; " | " &amp; Versions!$A$22 &amp; " | " &amp; Versions!$A$77 &amp; " | " &amp; Versions!$A$23 &amp; " | " &amp; Versions!$A$40 &amp; " | " &amp; Versions!$A$41</f>
         <v>@PLAN_VERSION | @PLAN_VERSION.v.LYR | @PLAN_VERSION.v.LYR% | @PLAN_VERSION.%.TOTAL.YEAR | @PLAN_VERSION.v.MFP | @PLAN_VERSION.v.MFP% | MFP | MWF | LYR | PYR | MF.v.MWF | LYR.v.PYR | MF.v.MWF% | LYR.v.PYR% | LYR.%.TOTAL.YEAR | MFP.%.TOTAL.YEAR</v>
       </c>
-      <c r="H18" t="b">
-        <v>1</v>
-      </c>
-      <c r="J18" t="str">
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" t="str">
         <f>ViewGroups!$A$122</f>
         <v>Fcst Merch Profit Views</v>
       </c>
-      <c r="K18" t="str">
+      <c r="L18" t="str">
         <f>CustomMenus!$A$22 &amp; " | " &amp; CustomMenus!$A$26</f>
         <v>mnuP_MWF2MF | mnuP_MF2CM</v>
       </c>
-      <c r="L18" t="str">
+      <c r="M18" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:13">
       <c r="A19" t="str">
         <f>Roles!$A$18</f>
         <v>Merch Profit Fcst</v>
@@ -58778,27 +58837,27 @@
         <f>RuleSet_FSProfit!$A$2</f>
         <v>FSProfit</v>
       </c>
-      <c r="G19" t="str">
+      <c r="H19" t="str">
         <f>DynamicMembers!$B$2 &amp; " | " &amp; DynamicMembers!$B$3 &amp; " | " &amp; DynamicMembers!$B$4 &amp; " | " &amp; DynamicMembers!$B$5 &amp; " | " &amp; DynamicMembers!$B$6 &amp; " | " &amp; DynamicMembers!$B$7 &amp; " | " &amp; Versions!$A$7 &amp; " | " &amp; Versions!$A$47 &amp; " | " &amp; Versions!$A$46 &amp; " | " &amp; Versions!$A$8 &amp; " | " &amp; Versions!$A$9 &amp; " | " &amp; Versions!$A$56 &amp; " | " &amp; Versions!$A$57 &amp; " | " &amp; Versions!$A$22 &amp; " | " &amp; Versions!$A$71 &amp; " | " &amp; Versions!$A$72 &amp; " | " &amp; Versions!$A$23 &amp; " | " &amp; Versions!$A$40 &amp; " | " &amp; Versions!$A$41</f>
         <v>@PLAN_VERSION | @PLAN_VERSION.v.LYR | @PLAN_VERSION.v.LYR% | @PLAN_VERSION.%.TOTAL.YEAR | @PLAN_VERSION.v.MFP | @PLAN_VERSION.v.MFP% | MFP | CMSF | MF | LYR | PYR | MWF.v.CMSF | MWF.v.MF | LYR.v.PYR | MWF.v.CMSF% | MWF.v.MF% | LYR.v.PYR% | LYR.%.TOTAL.YEAR | MFP.%.TOTAL.YEAR</v>
       </c>
-      <c r="H19" t="b">
-        <v>1</v>
-      </c>
-      <c r="J19" t="str">
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" t="str">
         <f>ViewGroups!$A$122</f>
         <v>Fcst Merch Profit Views</v>
       </c>
-      <c r="K19" t="str">
+      <c r="L19" t="str">
         <f>CustomMenus!$A$20 &amp; " | " &amp; CustomMenus!$A$22 &amp; " | " &amp; CustomMenus!$A$24</f>
         <v>mnuP_CSF2MF | mnuP_MWF2MF | mnuP_MWF2CM</v>
       </c>
-      <c r="L19" t="str">
+      <c r="M19" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:13">
       <c r="A20" t="str">
         <f>Roles!$A$20</f>
         <v>Merch Profit Fcst by CM</v>
@@ -58821,27 +58880,27 @@
         <f>RuleSet_FSProfit!$A$2</f>
         <v>FSProfit</v>
       </c>
-      <c r="G20" t="str">
+      <c r="H20" t="str">
         <f>DynamicMembers!$B$2 &amp; " | " &amp; DynamicMembers!$B$3 &amp; " | " &amp; DynamicMembers!$B$4 &amp; " | " &amp; DynamicMembers!$B$5 &amp; " | " &amp; DynamicMembers!$B$6 &amp; " | " &amp; DynamicMembers!$B$7 &amp; " | " &amp; Versions!$A$7 &amp; " | " &amp; Versions!$A$45 &amp; " | " &amp; Versions!$A$8 &amp; " | " &amp; Versions!$A$9 &amp; " | " &amp; Versions!$A$62 &amp; " | " &amp; Versions!$A$22 &amp; " | " &amp; Versions!$A$77 &amp; " | " &amp; Versions!$A$23 &amp; " | " &amp; Versions!$A$40 &amp; " | " &amp; Versions!$A$41</f>
         <v>@PLAN_VERSION | @PLAN_VERSION.v.LYR | @PLAN_VERSION.v.LYR% | @PLAN_VERSION.%.TOTAL.YEAR | @PLAN_VERSION.v.MFP | @PLAN_VERSION.v.MFP% | MFP | MWF | LYR | PYR | MF.v.MWF | LYR.v.PYR | MF.v.MWF% | LYR.v.PYR% | LYR.%.TOTAL.YEAR | MFP.%.TOTAL.YEAR</v>
       </c>
-      <c r="H20" t="b">
-        <v>1</v>
-      </c>
-      <c r="J20" t="str">
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" t="str">
         <f>ViewGroups!$A$122</f>
         <v>Fcst Merch Profit Views</v>
       </c>
-      <c r="K20" t="str">
+      <c r="L20" t="str">
         <f>CustomMenus!$A$22 &amp; " | " &amp; CustomMenus!$A$26</f>
         <v>mnuP_MWF2MF | mnuP_MF2CM</v>
       </c>
-      <c r="L20" t="str">
+      <c r="M20" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:13">
       <c r="A21" t="str">
         <f>Roles!$A$20</f>
         <v>Merch Profit Fcst by CM</v>
@@ -58864,27 +58923,27 @@
         <f>RuleSet_FSProfit!$A$2</f>
         <v>FSProfit</v>
       </c>
-      <c r="G21" t="str">
+      <c r="H21" t="str">
         <f>DynamicMembers!$B$2 &amp; " | " &amp; DynamicMembers!$B$3 &amp; " | " &amp; DynamicMembers!$B$4 &amp; " | " &amp; DynamicMembers!$B$5 &amp; " | " &amp; DynamicMembers!$B$6 &amp; " | " &amp; DynamicMembers!$B$7 &amp; " | " &amp; Versions!$A$7 &amp; " | " &amp; Versions!$A$47 &amp; " | " &amp; Versions!$A$46 &amp; " | " &amp; Versions!$A$8 &amp; " | " &amp; Versions!$A$9 &amp; " | " &amp; Versions!$A$56 &amp; " | " &amp; Versions!$A$57 &amp; " | " &amp; Versions!$A$22 &amp; " | " &amp; Versions!$A$71 &amp; " | " &amp; Versions!$A$72 &amp; " | " &amp; Versions!$A$23 &amp; " | " &amp; Versions!$A$40 &amp; " | " &amp; Versions!$A$41</f>
         <v>@PLAN_VERSION | @PLAN_VERSION.v.LYR | @PLAN_VERSION.v.LYR% | @PLAN_VERSION.%.TOTAL.YEAR | @PLAN_VERSION.v.MFP | @PLAN_VERSION.v.MFP% | MFP | CMSF | MF | LYR | PYR | MWF.v.CMSF | MWF.v.MF | LYR.v.PYR | MWF.v.CMSF% | MWF.v.MF% | LYR.v.PYR% | LYR.%.TOTAL.YEAR | MFP.%.TOTAL.YEAR</v>
       </c>
-      <c r="H21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J21" t="str">
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" t="str">
         <f>ViewGroups!$A$122</f>
         <v>Fcst Merch Profit Views</v>
       </c>
-      <c r="K21" t="str">
+      <c r="L21" t="str">
         <f>CustomMenus!$A$20 &amp; " | " &amp; CustomMenus!$A$22 &amp; " | " &amp; CustomMenus!$A$24</f>
         <v>mnuP_CSF2MF | mnuP_MWF2MF | mnuP_MWF2CM</v>
       </c>
-      <c r="L21" t="str">
+      <c r="M21" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:13">
       <c r="A22" s="35" t="s">
         <v>57</v>
       </c>
@@ -58895,19 +58954,366 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AM4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:39" ht="60">
+      <c r="A1" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39">
+      <c r="A2" t="s">
+        <v>937</v>
+      </c>
+      <c r="B2" t="s">
+        <v>963</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>880</v>
+      </c>
+      <c r="L2" t="s">
+        <v>881</v>
+      </c>
+      <c r="M2" t="s">
+        <v>882</v>
+      </c>
+      <c r="N2" t="s">
+        <v>883</v>
+      </c>
+      <c r="O2" t="s">
+        <v>884</v>
+      </c>
+      <c r="P2" t="s">
+        <v>884</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>883</v>
+      </c>
+      <c r="R2" t="s">
+        <v>882</v>
+      </c>
+      <c r="S2" t="b">
+        <v>0</v>
+      </c>
+      <c r="T2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W2" t="b">
+        <v>0</v>
+      </c>
+      <c r="X2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>885</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>886</v>
+      </c>
+      <c r="AF2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>887</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>888</v>
+      </c>
+      <c r="AL2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39">
+      <c r="A3" t="s">
+        <v>878</v>
+      </c>
+      <c r="B3" t="s">
+        <v>879</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>880</v>
+      </c>
+      <c r="L3" t="s">
+        <v>881</v>
+      </c>
+      <c r="M3" t="s">
+        <v>882</v>
+      </c>
+      <c r="N3" t="s">
+        <v>883</v>
+      </c>
+      <c r="O3" t="s">
+        <v>884</v>
+      </c>
+      <c r="P3" t="s">
+        <v>884</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>883</v>
+      </c>
+      <c r="R3" t="s">
+        <v>882</v>
+      </c>
+      <c r="S3" t="b">
+        <v>0</v>
+      </c>
+      <c r="T3" t="b">
+        <v>0</v>
+      </c>
+      <c r="W3" t="b">
+        <v>0</v>
+      </c>
+      <c r="X3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>885</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>886</v>
+      </c>
+      <c r="AF3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>887</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>888</v>
+      </c>
+      <c r="AL3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39">
+      <c r="A4" s="46" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -59098,7 +59504,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -59344,7 +59750,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -59481,7 +59887,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -59629,7 +60035,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -59683,8 +60089,55 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="45">
+      <c r="A1" s="44" t="s">
+        <v>952</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>953</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>955</v>
+      </c>
+      <c r="B2" t="s">
+        <v>832</v>
+      </c>
+      <c r="C2" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="C3" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="45" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -60188,12 +60641,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H83"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -60204,10 +60657,11 @@
     <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
         <v>58</v>
       </c>
@@ -60229,11 +60683,14 @@
       <c r="G1" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="44" t="s">
+        <v>959</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -60241,7 +60698,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>160</v>
       </c>
@@ -60249,7 +60706,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>162</v>
       </c>
@@ -60257,7 +60714,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>163</v>
       </c>
@@ -60265,7 +60722,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>164</v>
       </c>
@@ -60273,7 +60730,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>165</v>
       </c>
@@ -60281,7 +60738,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>166</v>
       </c>
@@ -60289,7 +60746,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>167</v>
       </c>
@@ -60297,7 +60754,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>168</v>
       </c>
@@ -60316,7 +60773,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>171</v>
       </c>
@@ -60335,7 +60792,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>172</v>
       </c>
@@ -60354,7 +60811,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>173</v>
       </c>
@@ -60373,7 +60830,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>174</v>
       </c>
@@ -60392,7 +60849,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>175</v>
       </c>
@@ -60411,7 +60868,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>176</v>
       </c>
@@ -60430,7 +60887,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>177</v>
       </c>
@@ -60449,7 +60906,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>178</v>
       </c>
@@ -60468,7 +60925,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>179</v>
       </c>
@@ -60487,7 +60944,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>180</v>
       </c>
@@ -60506,7 +60963,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>181</v>
       </c>
@@ -60525,7 +60982,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>182</v>
       </c>
@@ -60544,7 +61001,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>183</v>
       </c>
@@ -60562,12 +61019,12 @@
       <c r="E23" t="s">
         <v>184</v>
       </c>
-      <c r="H23" t="str">
+      <c r="I23" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>185</v>
       </c>
@@ -60585,12 +61042,12 @@
       <c r="E24" t="s">
         <v>170</v>
       </c>
-      <c r="H24" t="str">
+      <c r="I24" t="str">
         <f>NumericFormats!$A$16</f>
         <v>BP</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>186</v>
       </c>
@@ -60608,12 +61065,12 @@
       <c r="E25" t="s">
         <v>184</v>
       </c>
-      <c r="H25" t="str">
+      <c r="I25" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>187</v>
       </c>
@@ -60631,12 +61088,12 @@
       <c r="E26" t="s">
         <v>184</v>
       </c>
-      <c r="H26" t="str">
+      <c r="I26" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>188</v>
       </c>
@@ -60654,12 +61111,12 @@
       <c r="E27" t="s">
         <v>184</v>
       </c>
-      <c r="H27" t="str">
+      <c r="I27" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>189</v>
       </c>
@@ -60677,12 +61134,12 @@
       <c r="E28" t="s">
         <v>184</v>
       </c>
-      <c r="H28" t="str">
+      <c r="I28" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>190</v>
       </c>
@@ -60700,12 +61157,12 @@
       <c r="E29" t="s">
         <v>184</v>
       </c>
-      <c r="H29" t="str">
+      <c r="I29" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>191</v>
       </c>
@@ -60723,12 +61180,12 @@
       <c r="E30" t="s">
         <v>184</v>
       </c>
-      <c r="H30" t="str">
+      <c r="I30" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>192</v>
       </c>
@@ -60746,12 +61203,12 @@
       <c r="E31" t="s">
         <v>184</v>
       </c>
-      <c r="H31" t="str">
+      <c r="I31" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>193</v>
       </c>
@@ -60769,12 +61226,12 @@
       <c r="E32" t="s">
         <v>184</v>
       </c>
-      <c r="H32" t="str">
+      <c r="I32" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>194</v>
       </c>
@@ -60792,12 +61249,12 @@
       <c r="E33" t="s">
         <v>184</v>
       </c>
-      <c r="H33" t="str">
+      <c r="I33" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>195</v>
       </c>
@@ -60815,12 +61272,12 @@
       <c r="E34" t="s">
         <v>184</v>
       </c>
-      <c r="H34" t="str">
+      <c r="I34" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>196</v>
       </c>
@@ -60838,12 +61295,12 @@
       <c r="E35" t="s">
         <v>184</v>
       </c>
-      <c r="H35" t="str">
+      <c r="I35" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>197</v>
       </c>
@@ -60861,12 +61318,12 @@
       <c r="E36" t="s">
         <v>184</v>
       </c>
-      <c r="H36" t="str">
+      <c r="I36" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>198</v>
       </c>
@@ -60884,12 +61341,12 @@
       <c r="G37" t="s">
         <v>200</v>
       </c>
-      <c r="H37" t="str">
+      <c r="I37" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>201</v>
       </c>
@@ -60907,12 +61364,12 @@
       <c r="G38" t="s">
         <v>200</v>
       </c>
-      <c r="H38" t="str">
+      <c r="I38" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>202</v>
       </c>
@@ -60930,12 +61387,12 @@
       <c r="G39" t="s">
         <v>200</v>
       </c>
-      <c r="H39" t="str">
+      <c r="I39" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>203</v>
       </c>
@@ -60953,12 +61410,12 @@
       <c r="G40" t="s">
         <v>200</v>
       </c>
-      <c r="H40" t="str">
+      <c r="I40" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>204</v>
       </c>
@@ -60976,12 +61433,12 @@
       <c r="G41" t="s">
         <v>200</v>
       </c>
-      <c r="H41" t="str">
+      <c r="I41" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>205</v>
       </c>
@@ -60999,12 +61456,12 @@
       <c r="G42" t="s">
         <v>206</v>
       </c>
-      <c r="H42" t="str">
+      <c r="I42" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>207</v>
       </c>
@@ -61022,12 +61479,12 @@
       <c r="G43" t="s">
         <v>206</v>
       </c>
-      <c r="H43" t="str">
+      <c r="I43" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>209</v>
       </c>
@@ -61035,7 +61492,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>211</v>
       </c>
@@ -61043,7 +61500,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
         <v>208</v>
       </c>
@@ -61051,7 +61508,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
         <v>212</v>
       </c>
@@ -61059,7 +61516,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>213</v>
       </c>
@@ -61078,7 +61535,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>214</v>
       </c>
@@ -61097,7 +61554,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>215</v>
       </c>
@@ -61116,7 +61573,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>216</v>
       </c>
@@ -61135,7 +61592,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>217</v>
       </c>
@@ -61154,7 +61611,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
         <v>218</v>
       </c>
@@ -61173,7 +61630,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
         <v>219</v>
       </c>
@@ -61192,7 +61649,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>220</v>
       </c>
@@ -61211,7 +61668,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
         <v>221</v>
       </c>
@@ -61230,7 +61687,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:9">
       <c r="A57" t="s">
         <v>222</v>
       </c>
@@ -61249,7 +61706,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:9">
       <c r="A58" t="s">
         <v>223</v>
       </c>
@@ -61268,7 +61725,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:9">
       <c r="A59" t="s">
         <v>224</v>
       </c>
@@ -61287,7 +61744,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:9">
       <c r="A60" t="s">
         <v>225</v>
       </c>
@@ -61306,7 +61763,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:9">
       <c r="A61" t="s">
         <v>226</v>
       </c>
@@ -61325,7 +61782,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:9">
       <c r="A62" t="s">
         <v>227</v>
       </c>
@@ -61344,7 +61801,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:9">
       <c r="A63" t="s">
         <v>228</v>
       </c>
@@ -61362,12 +61819,12 @@
       <c r="E63" t="s">
         <v>184</v>
       </c>
-      <c r="H63" t="str">
+      <c r="I63" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:9">
       <c r="A64" t="s">
         <v>229</v>
       </c>
@@ -61385,12 +61842,12 @@
       <c r="E64" t="s">
         <v>184</v>
       </c>
-      <c r="H64" t="str">
+      <c r="I64" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:9">
       <c r="A65" t="s">
         <v>230</v>
       </c>
@@ -61408,12 +61865,12 @@
       <c r="E65" t="s">
         <v>184</v>
       </c>
-      <c r="H65" t="str">
+      <c r="I65" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:9">
       <c r="A66" t="s">
         <v>231</v>
       </c>
@@ -61431,12 +61888,12 @@
       <c r="E66" t="s">
         <v>184</v>
       </c>
-      <c r="H66" t="str">
+      <c r="I66" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:9">
       <c r="A67" t="s">
         <v>232</v>
       </c>
@@ -61454,12 +61911,12 @@
       <c r="E67" t="s">
         <v>184</v>
       </c>
-      <c r="H67" t="str">
+      <c r="I67" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:9">
       <c r="A68" t="s">
         <v>233</v>
       </c>
@@ -61477,12 +61934,12 @@
       <c r="E68" t="s">
         <v>184</v>
       </c>
-      <c r="H68" t="str">
+      <c r="I68" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:9">
       <c r="A69" t="s">
         <v>234</v>
       </c>
@@ -61500,12 +61957,12 @@
       <c r="E69" t="s">
         <v>184</v>
       </c>
-      <c r="H69" t="str">
+      <c r="I69" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:9">
       <c r="A70" t="s">
         <v>235</v>
       </c>
@@ -61523,12 +61980,12 @@
       <c r="E70" t="s">
         <v>184</v>
       </c>
-      <c r="H70" t="str">
+      <c r="I70" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:9">
       <c r="A71" t="s">
         <v>236</v>
       </c>
@@ -61546,12 +62003,12 @@
       <c r="E71" t="s">
         <v>184</v>
       </c>
-      <c r="H71" t="str">
+      <c r="I71" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:9">
       <c r="A72" t="s">
         <v>237</v>
       </c>
@@ -61569,12 +62026,12 @@
       <c r="E72" t="s">
         <v>184</v>
       </c>
-      <c r="H72" t="str">
+      <c r="I72" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:9">
       <c r="A73" t="s">
         <v>238</v>
       </c>
@@ -61592,12 +62049,12 @@
       <c r="E73" t="s">
         <v>184</v>
       </c>
-      <c r="H73" t="str">
+      <c r="I73" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:9">
       <c r="A74" t="s">
         <v>239</v>
       </c>
@@ -61615,12 +62072,12 @@
       <c r="E74" t="s">
         <v>184</v>
       </c>
-      <c r="H74" t="str">
+      <c r="I74" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:9">
       <c r="A75" t="s">
         <v>240</v>
       </c>
@@ -61638,12 +62095,12 @@
       <c r="E75" t="s">
         <v>184</v>
       </c>
-      <c r="H75" t="str">
+      <c r="I75" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:9">
       <c r="A76" t="s">
         <v>241</v>
       </c>
@@ -61661,12 +62118,12 @@
       <c r="E76" t="s">
         <v>184</v>
       </c>
-      <c r="H76" t="str">
+      <c r="I76" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:9">
       <c r="A77" t="s">
         <v>242</v>
       </c>
@@ -61684,12 +62141,12 @@
       <c r="E77" t="s">
         <v>184</v>
       </c>
-      <c r="H77" t="str">
+      <c r="I77" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:9">
       <c r="A78" t="s">
         <v>243</v>
       </c>
@@ -61707,12 +62164,12 @@
       <c r="G78" t="s">
         <v>200</v>
       </c>
-      <c r="H78" t="str">
+      <c r="I78" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:9">
       <c r="A79" t="s">
         <v>244</v>
       </c>
@@ -61730,12 +62187,12 @@
       <c r="G79" t="s">
         <v>200</v>
       </c>
-      <c r="H79" t="str">
+      <c r="I79" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:9">
       <c r="A80" t="s">
         <v>245</v>
       </c>
@@ -61753,12 +62210,12 @@
       <c r="G80" t="s">
         <v>200</v>
       </c>
-      <c r="H80" t="str">
+      <c r="I80" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:9">
       <c r="A81" t="s">
         <v>246</v>
       </c>
@@ -61776,12 +62233,12 @@
       <c r="G81" t="s">
         <v>206</v>
       </c>
-      <c r="H81" t="str">
+      <c r="I81" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:9">
       <c r="A82" t="s">
         <v>247</v>
       </c>
@@ -61799,12 +62256,12 @@
       <c r="G82" t="s">
         <v>206</v>
       </c>
-      <c r="H82" t="str">
+      <c r="I82" t="str">
         <f>NumericFormats!$A$17</f>
         <v>K%</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:9">
       <c r="A83" s="9" t="s">
         <v>57</v>
       </c>
@@ -61815,7 +62272,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -62644,7 +63101,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -62727,7 +63184,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -62823,7 +63280,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -62994,7 +63451,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
TTN 1533 - fix broken Junit Tests and clean up for PafAppsMigrationAction
</commit_message>
<xml_diff>
--- a/pace-base/test_files/2811-KatzExcelExport.xlsx
+++ b/pace-base/test_files/2811-KatzExcelExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="4125" windowWidth="21030" windowHeight="5670" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="105" yWindow="4125" windowWidth="21030" windowHeight="5670"/>
   </bookViews>
   <sheets>
     <sheet name="ApplicationDef" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3062" uniqueCount="964">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3064" uniqueCount="966">
   <si>
     <t>app id</t>
   </si>
@@ -39164,6 +39164,12 @@
   </si>
   <si>
     <t>Migration Print Style #1 - RENAME</t>
+  </si>
+  <si>
+    <t>enable multi-select role filter</t>
+  </si>
+  <si>
+    <t>app settings - is global user filtered multi-select</t>
   </si>
 </sst>
 </file>
@@ -39815,16 +39821,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM9"/>
+  <dimension ref="A1:AN9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:39" ht="150">
+    <row r="1" spans="1:40" ht="150">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -39846,104 +39852,107 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
+        <v>965</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:39">
+    <row r="2" spans="1:40">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -39959,187 +39968,190 @@
       <c r="H2" t="b">
         <v>0</v>
       </c>
-      <c r="L2" t="b">
-        <v>0</v>
-      </c>
-      <c r="M2" t="s">
-        <v>40</v>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" t="b">
+        <v>0</v>
       </c>
       <c r="N2" t="s">
         <v>40</v>
       </c>
       <c r="O2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" t="s">
         <v>41</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>43</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>44</v>
       </c>
-      <c r="S2" t="str">
-        <f>ApplicationDef!$AH$3</f>
+      <c r="T2" t="str">
+        <f>ApplicationDef!$AI$3</f>
         <v>CORP.HIERARCHY</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>46</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>47</v>
       </c>
-      <c r="W2" t="b">
-        <v>1</v>
-      </c>
       <c r="X2" t="b">
         <v>1</v>
       </c>
       <c r="Y2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z2" t="b">
         <v>0</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AA2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="s">
         <v>39</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>48</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>49</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>50</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>51</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>52</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>53</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>54</v>
       </c>
-      <c r="AI2" t="str">
+      <c r="AJ2" t="str">
+        <f>ApplicationDef!$AF$2</f>
+        <v>PLANTYPE</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM2">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40">
+      <c r="T3" t="str">
+        <f>ApplicationDef!$AG$2</f>
+        <v>LEDGER.TYPE</v>
+      </c>
+      <c r="U3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ3" t="str">
+        <f>ApplicationDef!$AH$2</f>
+        <v>YEAR</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40">
+      <c r="T4" t="str">
+        <f>ApplicationDef!$AC$2</f>
+        <v>MEASURE</v>
+      </c>
+      <c r="U4" t="s">
+        <v>46</v>
+      </c>
+      <c r="V4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ4" t="str">
+        <f>ApplicationDef!$AG$2</f>
+        <v>LEDGER.TYPE</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40">
+      <c r="T5" t="str">
+        <f>ApplicationDef!$AF$2</f>
+        <v>PLANTYPE</v>
+      </c>
+      <c r="U5" t="s">
+        <v>46</v>
+      </c>
+      <c r="V5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ5" t="str">
+        <f>ApplicationDef!$AC$2</f>
+        <v>MEASURE</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40">
+      <c r="T6" t="str">
+        <f>ApplicationDef!$AI$2</f>
+        <v>PRODUCT.HIERARCHY</v>
+      </c>
+      <c r="U6" t="s">
+        <v>46</v>
+      </c>
+      <c r="V6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ6" t="str">
         <f>ApplicationDef!$AE$2</f>
-        <v>PLANTYPE</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AL2">
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:39">
-      <c r="S3" t="str">
-        <f>ApplicationDef!$AF$2</f>
-        <v>LEDGER.TYPE</v>
-      </c>
-      <c r="T3" t="s">
+        <v>TIME</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40">
+      <c r="T7" t="str">
+        <f>ApplicationDef!$AE$2</f>
+        <v>TIME</v>
+      </c>
+      <c r="U7" t="s">
         <v>46</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V7" t="s">
         <v>47</v>
       </c>
-      <c r="AH3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI3" t="str">
-        <f>ApplicationDef!$AG$2</f>
+      <c r="AJ7" t="str">
+        <f>ApplicationDef!$AI$2</f>
+        <v>PRODUCT.HIERARCHY</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40">
+      <c r="T8" t="str">
+        <f>ApplicationDef!$AH$2</f>
         <v>YEAR</v>
       </c>
-    </row>
-    <row r="4" spans="1:39">
-      <c r="S4" t="str">
-        <f>ApplicationDef!$AB$2</f>
-        <v>MEASURE</v>
-      </c>
-      <c r="T4" t="s">
+      <c r="U8" t="s">
         <v>46</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V8" t="s">
         <v>47</v>
       </c>
-      <c r="AI4" t="str">
-        <f>ApplicationDef!$AF$2</f>
-        <v>LEDGER.TYPE</v>
-      </c>
-    </row>
-    <row r="5" spans="1:39">
-      <c r="S5" t="str">
-        <f>ApplicationDef!$AE$2</f>
-        <v>PLANTYPE</v>
-      </c>
-      <c r="T5" t="s">
-        <v>46</v>
-      </c>
-      <c r="U5" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI5" t="str">
-        <f>ApplicationDef!$AB$2</f>
-        <v>MEASURE</v>
-      </c>
-    </row>
-    <row r="6" spans="1:39">
-      <c r="S6" t="str">
-        <f>ApplicationDef!$AH$2</f>
-        <v>PRODUCT.HIERARCHY</v>
-      </c>
-      <c r="T6" t="s">
-        <v>46</v>
-      </c>
-      <c r="U6" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI6" t="str">
-        <f>ApplicationDef!$AD$2</f>
-        <v>TIME</v>
-      </c>
-    </row>
-    <row r="7" spans="1:39">
-      <c r="S7" t="str">
-        <f>ApplicationDef!$AD$2</f>
-        <v>TIME</v>
-      </c>
-      <c r="T7" t="s">
-        <v>46</v>
-      </c>
-      <c r="U7" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI7" t="str">
-        <f>ApplicationDef!$AH$2</f>
-        <v>PRODUCT.HIERARCHY</v>
-      </c>
-    </row>
-    <row r="8" spans="1:39">
-      <c r="S8" t="str">
-        <f>ApplicationDef!$AG$2</f>
-        <v>YEAR</v>
-      </c>
-      <c r="T8" t="s">
-        <v>46</v>
-      </c>
-      <c r="U8" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI8" t="str">
-        <f>ApplicationDef!$AH$3</f>
+      <c r="AJ8" t="str">
+        <f>ApplicationDef!$AI$3</f>
         <v>CORP.HIERARCHY</v>
       </c>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:40">
       <c r="A9" s="3" t="s">
         <v>57</v>
       </c>
@@ -40181,11 +40193,11 @@
         <v>350</v>
       </c>
       <c r="E1" s="20" t="str">
-        <f>ApplicationDef!$AH$2</f>
+        <f>ApplicationDef!$AI$2</f>
         <v>PRODUCT.HIERARCHY</v>
       </c>
       <c r="F1" s="20" t="str">
-        <f>ApplicationDef!$AH$3</f>
+        <f>ApplicationDef!$AI$3</f>
         <v>CORP.HIERARCHY</v>
       </c>
     </row>
@@ -41574,7 +41586,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="str">
-        <f>ApplicationDef!$AF$2</f>
+        <f>ApplicationDef!$AG$2</f>
         <v>LEDGER.TYPE</v>
       </c>
       <c r="B2" t="s">
@@ -58026,11 +58038,11 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -58044,19 +58056,20 @@
     <col min="7" max="7" width="29.42578125" customWidth="1"/>
     <col min="8" max="8" width="321.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="66" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="48.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="66" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="30">
+    <row r="1" spans="1:20" ht="30">
       <c r="A1" s="34" t="s">
         <v>350</v>
       </c>
@@ -58084,38 +58097,41 @@
       <c r="I1" s="34" t="s">
         <v>758</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="K1" s="34" t="s">
         <v>759</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="L1" s="34" t="s">
         <v>760</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="M1" s="34" t="s">
         <v>761</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="N1" s="34" t="s">
         <v>762</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="O1" s="34" t="s">
         <v>763</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="P1" s="34" t="s">
         <v>764</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="Q1" s="34" t="s">
         <v>765</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="R1" s="34" t="s">
         <v>766</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="S1" s="34" t="s">
         <v>767</v>
       </c>
-      <c r="S1" s="34" t="s">
+      <c r="T1" s="34" t="s">
         <v>768</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:20">
       <c r="A2" t="str">
         <f>Roles!$A$2</f>
         <v>Cat Mgr Merch Profit</v>
@@ -58145,20 +58161,20 @@
       <c r="I2" t="b">
         <v>1</v>
       </c>
-      <c r="K2" t="str">
+      <c r="L2" t="str">
         <f>ViewGroups!$A$40</f>
         <v>Cat Mgr Views</v>
       </c>
-      <c r="L2" t="str">
+      <c r="M2" t="str">
         <f>CustomMenus!$A$2 &amp; " | " &amp; CustomMenus!$A$4 &amp; " | " &amp; CustomMenus!$A$10 &amp; " | " &amp; CustomMenus!$A$12</f>
         <v>mnuP_LYR2WP | mnuP_CMWP2S | mnuP_MWP2CM | mnuP_MP2CM</v>
       </c>
-      <c r="M2" t="str">
+      <c r="N2" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:20">
       <c r="A3" t="str">
         <f>Roles!$A$3</f>
         <v>Cat Mgr Merch Profit Fcst</v>
@@ -58188,20 +58204,20 @@
       <c r="I3" t="b">
         <v>1</v>
       </c>
-      <c r="K3" t="str">
+      <c r="L3" t="str">
         <f>ViewGroups!$A$2</f>
         <v>Fcst Cat Mgr Views</v>
       </c>
-      <c r="L3" t="str">
+      <c r="M3" t="str">
         <f>CustomMenus!$A$18 &amp; " | " &amp; CustomMenus!$A$24 &amp; " | " &amp; CustomMenus!$A$26</f>
         <v>mnuP_CMWF2S | mnuP_MWF2CM | mnuP_MF2CM</v>
       </c>
-      <c r="M3" t="str">
+      <c r="N3" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:20">
       <c r="A4" t="str">
         <f>Roles!$A$4</f>
         <v>Consolidated Merch Profit</v>
@@ -58231,12 +58247,12 @@
       <c r="I4" t="b">
         <v>1</v>
       </c>
-      <c r="K4" t="str">
+      <c r="L4" t="str">
         <f>ViewGroups!$A$54</f>
         <v>Merch Profit Views</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:20">
       <c r="A5" t="str">
         <f>Roles!$A$4</f>
         <v>Consolidated Merch Profit</v>
@@ -58266,12 +58282,12 @@
       <c r="I5" t="b">
         <v>1</v>
       </c>
-      <c r="K5" t="str">
+      <c r="L5" t="str">
         <f>ViewGroups!$A$54</f>
         <v>Merch Profit Views</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:20">
       <c r="A6" t="str">
         <f>Roles!$A$6</f>
         <v>Consolidated Merch Profit by CM</v>
@@ -58301,12 +58317,12 @@
       <c r="I6" t="b">
         <v>1</v>
       </c>
-      <c r="K6" t="str">
+      <c r="L6" t="str">
         <f>ViewGroups!$A$54</f>
         <v>Merch Profit Views</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:20">
       <c r="A7" t="str">
         <f>Roles!$A$6</f>
         <v>Consolidated Merch Profit by CM</v>
@@ -58336,12 +58352,12 @@
       <c r="I7" t="b">
         <v>1</v>
       </c>
-      <c r="K7" t="str">
+      <c r="L7" t="str">
         <f>ViewGroups!$A$54</f>
         <v>Merch Profit Views</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:20">
       <c r="A8" t="str">
         <f>Roles!$A$8</f>
         <v>LYR Update</v>
@@ -58371,20 +58387,20 @@
       <c r="I8" t="b">
         <v>1</v>
       </c>
-      <c r="K8" t="str">
+      <c r="L8" t="str">
         <f>ViewGroups!$A$90</f>
         <v>LYR Update Views</v>
       </c>
-      <c r="L8" t="str">
+      <c r="M8" t="str">
         <f>CustomMenus!$A$14 &amp; " | " &amp; CustomMenus!$A$16</f>
         <v>mnuP_LYR2P | mnuP_LYR2PE</v>
       </c>
-      <c r="M8" t="str">
+      <c r="N8" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:20">
       <c r="A9" t="str">
         <f>Roles!$A$9</f>
         <v>LYR Update by CM</v>
@@ -58414,20 +58430,20 @@
       <c r="I9" t="b">
         <v>1</v>
       </c>
-      <c r="K9" t="str">
+      <c r="L9" t="str">
         <f>ViewGroups!$A$90</f>
         <v>LYR Update Views</v>
       </c>
-      <c r="L9" t="str">
+      <c r="M9" t="str">
         <f>CustomMenus!$A$14 &amp; " | " &amp; CustomMenus!$A$16</f>
         <v>mnuP_LYR2P | mnuP_LYR2PE</v>
       </c>
-      <c r="M9" t="str">
+      <c r="N9" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:20">
       <c r="A10" t="str">
         <f>Roles!$A$10</f>
         <v>Merch Profit - COM Stores</v>
@@ -58457,20 +58473,20 @@
       <c r="I10" t="b">
         <v>1</v>
       </c>
-      <c r="K10" t="str">
+      <c r="L10" t="str">
         <f>ViewGroups!$A$54</f>
         <v>Merch Profit Views</v>
       </c>
-      <c r="L10" t="str">
+      <c r="M10" t="str">
         <f>CustomMenus!$A$2 &amp; " | " &amp; CustomMenus!$A$8 &amp; " | " &amp; CustomMenus!$A$12</f>
         <v>mnuP_LYR2WP | mnuP_MWP2MP | mnuP_MP2CM</v>
       </c>
-      <c r="M10" t="str">
+      <c r="N10" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:20">
       <c r="A11" t="str">
         <f>Roles!$A$10</f>
         <v>Merch Profit - COM Stores</v>
@@ -58500,20 +58516,20 @@
       <c r="I11" t="b">
         <v>1</v>
       </c>
-      <c r="K11" t="str">
+      <c r="L11" t="str">
         <f>ViewGroups!$A$54</f>
         <v>Merch Profit Views</v>
       </c>
-      <c r="L11" t="str">
+      <c r="M11" t="str">
         <f>CustomMenus!$A$2 &amp; " | " &amp; CustomMenus!$A$6 &amp; " | " &amp; CustomMenus!$A$8 &amp; " | " &amp; CustomMenus!$A$10</f>
         <v>mnuP_LYR2WP | mnuP_CSP2MW | mnuP_MWP2MP | mnuP_MWP2CM</v>
       </c>
-      <c r="M11" t="str">
+      <c r="N11" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:20">
       <c r="A12" t="str">
         <f>Roles!$A$12</f>
         <v>Merch Profit - Not COM Stores</v>
@@ -58543,20 +58559,20 @@
       <c r="I12" t="b">
         <v>1</v>
       </c>
-      <c r="K12" t="str">
+      <c r="L12" t="str">
         <f>ViewGroups!$A$108</f>
         <v>Not-Comp Views</v>
       </c>
-      <c r="L12" t="str">
+      <c r="M12" t="str">
         <f>CustomMenus!$A$8</f>
         <v>mnuP_MWP2MP</v>
       </c>
-      <c r="M12" t="str">
+      <c r="N12" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:20">
       <c r="A13" t="str">
         <f>Roles!$A$12</f>
         <v>Merch Profit - Not COM Stores</v>
@@ -58586,20 +58602,20 @@
       <c r="I13" t="b">
         <v>1</v>
       </c>
-      <c r="K13" t="str">
+      <c r="L13" t="str">
         <f>ViewGroups!$A$108</f>
         <v>Not-Comp Views</v>
       </c>
-      <c r="L13" t="str">
+      <c r="M13" t="str">
         <f>CustomMenus!$A$8</f>
         <v>mnuP_MWP2MP</v>
       </c>
-      <c r="M13" t="str">
+      <c r="N13" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:20">
       <c r="A14" t="str">
         <f>Roles!$A$14</f>
         <v>Merch Profit by CM - COM Stores</v>
@@ -58629,20 +58645,20 @@
       <c r="I14" t="b">
         <v>1</v>
       </c>
-      <c r="K14" t="str">
+      <c r="L14" t="str">
         <f>ViewGroups!$A$54</f>
         <v>Merch Profit Views</v>
       </c>
-      <c r="L14" t="str">
+      <c r="M14" t="str">
         <f>CustomMenus!$A$2 &amp; " | " &amp; CustomMenus!$A$8 &amp; " | " &amp; CustomMenus!$A$12</f>
         <v>mnuP_LYR2WP | mnuP_MWP2MP | mnuP_MP2CM</v>
       </c>
-      <c r="M14" t="str">
+      <c r="N14" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:20">
       <c r="A15" t="str">
         <f>Roles!$A$14</f>
         <v>Merch Profit by CM - COM Stores</v>
@@ -58672,20 +58688,20 @@
       <c r="I15" t="b">
         <v>1</v>
       </c>
-      <c r="K15" t="str">
+      <c r="L15" t="str">
         <f>ViewGroups!$A$54</f>
         <v>Merch Profit Views</v>
       </c>
-      <c r="L15" t="str">
+      <c r="M15" t="str">
         <f>CustomMenus!$A$2 &amp; " | " &amp; CustomMenus!$A$6 &amp; " | " &amp; CustomMenus!$A$8 &amp; " | " &amp; CustomMenus!$A$10</f>
         <v>mnuP_LYR2WP | mnuP_CSP2MW | mnuP_MWP2MP | mnuP_MWP2CM</v>
       </c>
-      <c r="M15" t="str">
+      <c r="N15" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:20">
       <c r="A16" t="str">
         <f>Roles!$A$16</f>
         <v>Merch Profit by CM - Not COM Stores</v>
@@ -58715,20 +58731,20 @@
       <c r="I16" t="b">
         <v>1</v>
       </c>
-      <c r="K16" t="str">
+      <c r="L16" t="str">
         <f>ViewGroups!$A$108</f>
         <v>Not-Comp Views</v>
       </c>
-      <c r="L16" t="str">
+      <c r="M16" t="str">
         <f>CustomMenus!$A$8</f>
         <v>mnuP_MWP2MP</v>
       </c>
-      <c r="M16" t="str">
+      <c r="N16" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:14">
       <c r="A17" t="str">
         <f>Roles!$A$16</f>
         <v>Merch Profit by CM - Not COM Stores</v>
@@ -58758,20 +58774,20 @@
       <c r="I17" t="b">
         <v>1</v>
       </c>
-      <c r="K17" t="str">
+      <c r="L17" t="str">
         <f>ViewGroups!$A$108</f>
         <v>Not-Comp Views</v>
       </c>
-      <c r="L17" t="str">
+      <c r="M17" t="str">
         <f>CustomMenus!$A$8</f>
         <v>mnuP_MWP2MP</v>
       </c>
-      <c r="M17" t="str">
+      <c r="N17" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:14">
       <c r="A18" t="str">
         <f>Roles!$A$18</f>
         <v>Merch Profit Fcst</v>
@@ -58801,20 +58817,20 @@
       <c r="I18" t="b">
         <v>1</v>
       </c>
-      <c r="K18" t="str">
+      <c r="L18" t="str">
         <f>ViewGroups!$A$122</f>
         <v>Fcst Merch Profit Views</v>
       </c>
-      <c r="L18" t="str">
+      <c r="M18" t="str">
         <f>CustomMenus!$A$22 &amp; " | " &amp; CustomMenus!$A$26</f>
         <v>mnuP_MWF2MF | mnuP_MF2CM</v>
       </c>
-      <c r="M18" t="str">
+      <c r="N18" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:14">
       <c r="A19" t="str">
         <f>Roles!$A$18</f>
         <v>Merch Profit Fcst</v>
@@ -58844,20 +58860,20 @@
       <c r="I19" t="b">
         <v>1</v>
       </c>
-      <c r="K19" t="str">
+      <c r="L19" t="str">
         <f>ViewGroups!$A$122</f>
         <v>Fcst Merch Profit Views</v>
       </c>
-      <c r="L19" t="str">
+      <c r="M19" t="str">
         <f>CustomMenus!$A$20 &amp; " | " &amp; CustomMenus!$A$22 &amp; " | " &amp; CustomMenus!$A$24</f>
         <v>mnuP_CSF2MF | mnuP_MWF2MF | mnuP_MWF2CM</v>
       </c>
-      <c r="M19" t="str">
+      <c r="N19" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:14">
       <c r="A20" t="str">
         <f>Roles!$A$20</f>
         <v>Merch Profit Fcst by CM</v>
@@ -58887,20 +58903,20 @@
       <c r="I20" t="b">
         <v>1</v>
       </c>
-      <c r="K20" t="str">
+      <c r="L20" t="str">
         <f>ViewGroups!$A$122</f>
         <v>Fcst Merch Profit Views</v>
       </c>
-      <c r="L20" t="str">
+      <c r="M20" t="str">
         <f>CustomMenus!$A$22 &amp; " | " &amp; CustomMenus!$A$26</f>
         <v>mnuP_MWF2MF | mnuP_MF2CM</v>
       </c>
-      <c r="M20" t="str">
+      <c r="N20" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:14">
       <c r="A21" t="str">
         <f>Roles!$A$20</f>
         <v>Merch Profit Fcst by CM</v>
@@ -58930,20 +58946,20 @@
       <c r="I21" t="b">
         <v>1</v>
       </c>
-      <c r="K21" t="str">
+      <c r="L21" t="str">
         <f>ViewGroups!$A$122</f>
         <v>Fcst Merch Profit Views</v>
       </c>
-      <c r="L21" t="str">
+      <c r="M21" t="str">
         <f>CustomMenus!$A$20 &amp; " | " &amp; CustomMenus!$A$22 &amp; " | " &amp; CustomMenus!$A$24</f>
         <v>mnuP_CSF2MF | mnuP_MWF2MF | mnuP_MWF2CM</v>
       </c>
-      <c r="M21" t="str">
+      <c r="N21" t="str">
         <f>CustomMenus!$A$28</f>
         <v>mnuP_AGG</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:14">
       <c r="A22" s="35" t="s">
         <v>57</v>
       </c>
@@ -59348,7 +59364,7 @@
         <v>771</v>
       </c>
       <c r="B2" t="str">
-        <f>ApplicationDef!$AH$3</f>
+        <f>ApplicationDef!$AI$3</f>
         <v>CORP.HIERARCHY</v>
       </c>
       <c r="C2" t="b">
@@ -59363,7 +59379,7 @@
         <v>773</v>
       </c>
       <c r="B3" t="str">
-        <f>ApplicationDef!$AH$3</f>
+        <f>ApplicationDef!$AI$3</f>
         <v>CORP.HIERARCHY</v>
       </c>
       <c r="C3" t="b">
@@ -59378,7 +59394,7 @@
         <v>775</v>
       </c>
       <c r="B4" t="str">
-        <f>ApplicationDef!$AF$2</f>
+        <f>ApplicationDef!$AG$2</f>
         <v>LEDGER.TYPE</v>
       </c>
       <c r="C4" t="b">
@@ -59393,7 +59409,7 @@
         <v>777</v>
       </c>
       <c r="B5" t="str">
-        <f>ApplicationDef!$AF$2</f>
+        <f>ApplicationDef!$AG$2</f>
         <v>LEDGER.TYPE</v>
       </c>
       <c r="C5" t="b">
@@ -59408,7 +59424,7 @@
         <v>779</v>
       </c>
       <c r="B6" t="str">
-        <f>ApplicationDef!$AB$2</f>
+        <f>ApplicationDef!$AC$2</f>
         <v>MEASURE</v>
       </c>
       <c r="C6" t="b">
@@ -59423,7 +59439,7 @@
         <v>781</v>
       </c>
       <c r="B7" t="str">
-        <f>ApplicationDef!$AB$2</f>
+        <f>ApplicationDef!$AC$2</f>
         <v>MEASURE</v>
       </c>
       <c r="C7" t="b">
@@ -59438,7 +59454,7 @@
         <v>783</v>
       </c>
       <c r="B8" t="str">
-        <f>ApplicationDef!$AH$2</f>
+        <f>ApplicationDef!$AI$2</f>
         <v>PRODUCT.HIERARCHY</v>
       </c>
       <c r="C8" t="b">
@@ -59453,7 +59469,7 @@
         <v>785</v>
       </c>
       <c r="B9" t="str">
-        <f>ApplicationDef!$AH$2</f>
+        <f>ApplicationDef!$AI$2</f>
         <v>PRODUCT.HIERARCHY</v>
       </c>
       <c r="C9" t="b">
@@ -59468,7 +59484,7 @@
         <v>787</v>
       </c>
       <c r="B10" t="str">
-        <f>ApplicationDef!$AD$2</f>
+        <f>ApplicationDef!$AE$2</f>
         <v>TIME</v>
       </c>
       <c r="C10" t="b">
@@ -59483,7 +59499,7 @@
         <v>789</v>
       </c>
       <c r="B11" t="str">
-        <f>ApplicationDef!$AD$2</f>
+        <f>ApplicationDef!$AE$2</f>
         <v>TIME</v>
       </c>
       <c r="C11" t="b">
@@ -59961,7 +59977,7 @@
         <v>829</v>
       </c>
       <c r="D4" t="str">
-        <f>ApplicationDef!$AD$2</f>
+        <f>ApplicationDef!$AE$2</f>
         <v>TIME</v>
       </c>
       <c r="E4" t="b">
@@ -59973,7 +59989,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="D5" t="str">
-        <f>ApplicationDef!$AG$2</f>
+        <f>ApplicationDef!$AH$2</f>
         <v>YEAR</v>
       </c>
     </row>
@@ -60008,7 +60024,7 @@
         <v>834</v>
       </c>
       <c r="D7" t="str">
-        <f>ApplicationDef!$AD$2</f>
+        <f>ApplicationDef!$AE$2</f>
         <v>TIME</v>
       </c>
       <c r="E7" t="b">
@@ -60020,7 +60036,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="D8" t="str">
-        <f>ApplicationDef!$AG$2</f>
+        <f>ApplicationDef!$AH$2</f>
         <v>YEAR</v>
       </c>
     </row>
@@ -60644,7 +60660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
@@ -61335,7 +61351,7 @@
         <v>CMWP</v>
       </c>
       <c r="F37" t="str">
-        <f>ApplicationDef!$AD$2</f>
+        <f>ApplicationDef!$AE$2</f>
         <v>TIME</v>
       </c>
       <c r="G37" t="s">
@@ -61358,7 +61374,7 @@
         <v>MWP</v>
       </c>
       <c r="F38" t="str">
-        <f>ApplicationDef!$AD$2</f>
+        <f>ApplicationDef!$AE$2</f>
         <v>TIME</v>
       </c>
       <c r="G38" t="s">
@@ -61381,7 +61397,7 @@
         <v>MP</v>
       </c>
       <c r="F39" t="str">
-        <f>ApplicationDef!$AD$2</f>
+        <f>ApplicationDef!$AE$2</f>
         <v>TIME</v>
       </c>
       <c r="G39" t="s">
@@ -61404,7 +61420,7 @@
         <v>LYR</v>
       </c>
       <c r="F40" t="str">
-        <f>ApplicationDef!$AD$2</f>
+        <f>ApplicationDef!$AE$2</f>
         <v>TIME</v>
       </c>
       <c r="G40" t="s">
@@ -61427,7 +61443,7 @@
         <v>MFP</v>
       </c>
       <c r="F41" t="str">
-        <f>ApplicationDef!$AD$2</f>
+        <f>ApplicationDef!$AE$2</f>
         <v>TIME</v>
       </c>
       <c r="G41" t="s">
@@ -61450,7 +61466,7 @@
         <v>MWP</v>
       </c>
       <c r="F42" t="str">
-        <f>ApplicationDef!$AH$2</f>
+        <f>ApplicationDef!$AI$2</f>
         <v>PRODUCT.HIERARCHY</v>
       </c>
       <c r="G42" t="s">
@@ -61473,7 +61489,7 @@
         <v>MF</v>
       </c>
       <c r="F43" t="str">
-        <f>ApplicationDef!$AH$2</f>
+        <f>ApplicationDef!$AI$2</f>
         <v>PRODUCT.HIERARCHY</v>
       </c>
       <c r="G43" t="s">
@@ -62158,7 +62174,7 @@
         <v>CMWF</v>
       </c>
       <c r="F78" t="str">
-        <f>ApplicationDef!$AD$2</f>
+        <f>ApplicationDef!$AE$2</f>
         <v>TIME</v>
       </c>
       <c r="G78" t="s">
@@ -62181,7 +62197,7 @@
         <v>MWF</v>
       </c>
       <c r="F79" t="str">
-        <f>ApplicationDef!$AD$2</f>
+        <f>ApplicationDef!$AE$2</f>
         <v>TIME</v>
       </c>
       <c r="G79" t="s">
@@ -62204,7 +62220,7 @@
         <v>MF</v>
       </c>
       <c r="F80" t="str">
-        <f>ApplicationDef!$AD$2</f>
+        <f>ApplicationDef!$AE$2</f>
         <v>TIME</v>
       </c>
       <c r="G80" t="s">
@@ -62227,7 +62243,7 @@
         <v>MWF</v>
       </c>
       <c r="F81" t="str">
-        <f>ApplicationDef!$AH$2</f>
+        <f>ApplicationDef!$AI$2</f>
         <v>PRODUCT.HIERARCHY</v>
       </c>
       <c r="G81" t="s">
@@ -62250,7 +62266,7 @@
         <v>MF</v>
       </c>
       <c r="F82" t="str">
-        <f>ApplicationDef!$AH$2</f>
+        <f>ApplicationDef!$AI$2</f>
         <v>PRODUCT.HIERARCHY</v>
       </c>
       <c r="G82" t="s">
@@ -63140,7 +63156,7 @@
         <v>306</v>
       </c>
       <c r="B2" t="str">
-        <f>ApplicationDef!$AD$2</f>
+        <f>ApplicationDef!$AE$2</f>
         <v>TIME</v>
       </c>
       <c r="C2" t="s">
@@ -63159,7 +63175,7 @@
         <v>308</v>
       </c>
       <c r="B3" t="str">
-        <f>ApplicationDef!$AD$2</f>
+        <f>ApplicationDef!$AE$2</f>
         <v>TIME</v>
       </c>
       <c r="C3" t="s">

</xml_diff>

<commit_message>
TTN-1862: Week 53 Support
</commit_message>
<xml_diff>
--- a/pace-base/test_files/2811-KatzExcelExport.xlsx
+++ b/pace-base/test_files/2811-KatzExcelExport.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3067" uniqueCount="970">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3071" uniqueCount="973">
   <si>
     <t>app id</t>
   </si>
@@ -39183,6 +39183,15 @@
   </si>
   <si>
     <t>WK52</t>
+  </si>
+  <si>
+    <t>app colors - non plannable protected color</t>
+  </si>
+  <si>
+    <t>app colors - forward plannable protected color</t>
+  </si>
+  <si>
+    <t>FF8080</t>
   </si>
 </sst>
 </file>
@@ -39891,16 +39900,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO9"/>
+  <dimension ref="A1:AQ9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O1" sqref="O1:P1048576"/>
+      <selection pane="bottomLeft" activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:41" ht="150">
+    <row r="1" spans="1:43" ht="150">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -39949,83 +39958,89 @@
       <c r="P1" s="49" t="s">
         <v>966</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="49" t="s">
+        <v>970</v>
+      </c>
+      <c r="R1" s="49" t="s">
+        <v>971</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:41">
+    <row r="2" spans="1:43">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -40054,180 +40069,186 @@
         <v>968</v>
       </c>
       <c r="Q2" t="s">
+        <v>132</v>
+      </c>
+      <c r="R2" t="s">
+        <v>972</v>
+      </c>
+      <c r="S2" t="s">
         <v>38</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>39</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>40</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V2" t="s">
         <v>41</v>
       </c>
-      <c r="U2" t="str">
-        <f>ApplicationDef!$AJ$3</f>
+      <c r="W2" t="str">
+        <f>ApplicationDef!$AL$3</f>
         <v>CORP.HIERARCHY</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>43</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>44</v>
       </c>
-      <c r="Y2" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z2" t="b">
-        <v>1</v>
-      </c>
       <c r="AA2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="s">
         <v>37</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AF2" t="s">
         <v>45</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AG2" t="s">
         <v>46</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AH2" t="s">
         <v>47</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AI2" t="s">
         <v>48</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AJ2" t="s">
         <v>49</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AK2" t="s">
         <v>50</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AL2" t="s">
         <v>51</v>
       </c>
-      <c r="AK2" t="str">
-        <f>ApplicationDef!$AG$2</f>
+      <c r="AM2" t="str">
+        <f>ApplicationDef!$AI$2</f>
         <v>PLANTYPE</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AN2" t="s">
         <v>52</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AO2" t="s">
         <v>53</v>
       </c>
-      <c r="AN2">
+      <c r="AP2">
         <v>60000</v>
       </c>
     </row>
-    <row r="3" spans="1:41">
+    <row r="3" spans="1:43">
       <c r="P3" t="s">
         <v>969</v>
       </c>
-      <c r="U3" t="str">
+      <c r="W3" t="str">
+        <f>ApplicationDef!$AJ$2</f>
+        <v>LEDGER.TYPE</v>
+      </c>
+      <c r="X3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM3" t="str">
+        <f>ApplicationDef!$AK$2</f>
+        <v>YEAR</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43">
+      <c r="W4" t="str">
+        <f>ApplicationDef!$AF$2</f>
+        <v>MEASURE</v>
+      </c>
+      <c r="X4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM4" t="str">
+        <f>ApplicationDef!$AJ$2</f>
+        <v>LEDGER.TYPE</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43">
+      <c r="W5" t="str">
+        <f>ApplicationDef!$AI$2</f>
+        <v>PLANTYPE</v>
+      </c>
+      <c r="X5" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM5" t="str">
+        <f>ApplicationDef!$AF$2</f>
+        <v>MEASURE</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43">
+      <c r="W6" t="str">
+        <f>ApplicationDef!$AL$2</f>
+        <v>PRODUCT.HIERARCHY</v>
+      </c>
+      <c r="X6" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM6" t="str">
         <f>ApplicationDef!$AH$2</f>
-        <v>LEDGER.TYPE</v>
-      </c>
-      <c r="V3" t="s">
+        <v>TIME</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43">
+      <c r="W7" t="str">
+        <f>ApplicationDef!$AH$2</f>
+        <v>TIME</v>
+      </c>
+      <c r="X7" t="s">
         <v>43</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Y7" t="s">
         <v>44</v>
       </c>
-      <c r="AJ3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AK3" t="str">
-        <f>ApplicationDef!$AI$2</f>
+      <c r="AM7" t="str">
+        <f>ApplicationDef!$AL$2</f>
+        <v>PRODUCT.HIERARCHY</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43">
+      <c r="W8" t="str">
+        <f>ApplicationDef!$AK$2</f>
         <v>YEAR</v>
       </c>
-    </row>
-    <row r="4" spans="1:41">
-      <c r="U4" t="str">
-        <f>ApplicationDef!$AD$2</f>
-        <v>MEASURE</v>
-      </c>
-      <c r="V4" t="s">
+      <c r="X8" t="s">
         <v>43</v>
       </c>
-      <c r="W4" t="s">
+      <c r="Y8" t="s">
         <v>44</v>
       </c>
-      <c r="AK4" t="str">
-        <f>ApplicationDef!$AH$2</f>
-        <v>LEDGER.TYPE</v>
-      </c>
-    </row>
-    <row r="5" spans="1:41">
-      <c r="U5" t="str">
-        <f>ApplicationDef!$AG$2</f>
-        <v>PLANTYPE</v>
-      </c>
-      <c r="V5" t="s">
-        <v>43</v>
-      </c>
-      <c r="W5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AK5" t="str">
-        <f>ApplicationDef!$AD$2</f>
-        <v>MEASURE</v>
-      </c>
-    </row>
-    <row r="6" spans="1:41">
-      <c r="U6" t="str">
-        <f>ApplicationDef!$AJ$2</f>
-        <v>PRODUCT.HIERARCHY</v>
-      </c>
-      <c r="V6" t="s">
-        <v>43</v>
-      </c>
-      <c r="W6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AK6" t="str">
-        <f>ApplicationDef!$AF$2</f>
-        <v>TIME</v>
-      </c>
-    </row>
-    <row r="7" spans="1:41">
-      <c r="U7" t="str">
-        <f>ApplicationDef!$AF$2</f>
-        <v>TIME</v>
-      </c>
-      <c r="V7" t="s">
-        <v>43</v>
-      </c>
-      <c r="W7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AK7" t="str">
-        <f>ApplicationDef!$AJ$2</f>
-        <v>PRODUCT.HIERARCHY</v>
-      </c>
-    </row>
-    <row r="8" spans="1:41">
-      <c r="U8" t="str">
-        <f>ApplicationDef!$AI$2</f>
-        <v>YEAR</v>
-      </c>
-      <c r="V8" t="s">
-        <v>43</v>
-      </c>
-      <c r="W8" t="s">
-        <v>44</v>
-      </c>
-      <c r="AK8" t="str">
-        <f>ApplicationDef!$AJ$3</f>
+      <c r="AM8" t="str">
+        <f>ApplicationDef!$AL$3</f>
         <v>CORP.HIERARCHY</v>
       </c>
     </row>
-    <row r="9" spans="1:41">
+    <row r="9" spans="1:43">
       <c r="A9" s="3" t="s">
         <v>54</v>
       </c>
@@ -40269,11 +40290,11 @@
         <v>347</v>
       </c>
       <c r="E1" s="20" t="str">
-        <f>ApplicationDef!$AJ$2</f>
+        <f>ApplicationDef!$AL$2</f>
         <v>PRODUCT.HIERARCHY</v>
       </c>
       <c r="F1" s="20" t="str">
-        <f>ApplicationDef!$AJ$3</f>
+        <f>ApplicationDef!$AL$3</f>
         <v>CORP.HIERARCHY</v>
       </c>
     </row>
@@ -41662,7 +41683,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="str">
-        <f>ApplicationDef!$AH$2</f>
+        <f>ApplicationDef!$AJ$2</f>
         <v>LEDGER.TYPE</v>
       </c>
       <c r="B2" t="s">
@@ -59442,7 +59463,7 @@
         <v>768</v>
       </c>
       <c r="B2" t="str">
-        <f>ApplicationDef!$AJ$3</f>
+        <f>ApplicationDef!$AL$3</f>
         <v>CORP.HIERARCHY</v>
       </c>
       <c r="C2" t="b">
@@ -59457,7 +59478,7 @@
         <v>770</v>
       </c>
       <c r="B3" t="str">
-        <f>ApplicationDef!$AJ$3</f>
+        <f>ApplicationDef!$AL$3</f>
         <v>CORP.HIERARCHY</v>
       </c>
       <c r="C3" t="b">
@@ -59472,7 +59493,7 @@
         <v>772</v>
       </c>
       <c r="B4" t="str">
-        <f>ApplicationDef!$AH$2</f>
+        <f>ApplicationDef!$AJ$2</f>
         <v>LEDGER.TYPE</v>
       </c>
       <c r="C4" t="b">
@@ -59487,7 +59508,7 @@
         <v>774</v>
       </c>
       <c r="B5" t="str">
-        <f>ApplicationDef!$AH$2</f>
+        <f>ApplicationDef!$AJ$2</f>
         <v>LEDGER.TYPE</v>
       </c>
       <c r="C5" t="b">
@@ -59502,7 +59523,7 @@
         <v>776</v>
       </c>
       <c r="B6" t="str">
-        <f>ApplicationDef!$AD$2</f>
+        <f>ApplicationDef!$AF$2</f>
         <v>MEASURE</v>
       </c>
       <c r="C6" t="b">
@@ -59517,7 +59538,7 @@
         <v>778</v>
       </c>
       <c r="B7" t="str">
-        <f>ApplicationDef!$AD$2</f>
+        <f>ApplicationDef!$AF$2</f>
         <v>MEASURE</v>
       </c>
       <c r="C7" t="b">
@@ -59532,7 +59553,7 @@
         <v>780</v>
       </c>
       <c r="B8" t="str">
-        <f>ApplicationDef!$AJ$2</f>
+        <f>ApplicationDef!$AL$2</f>
         <v>PRODUCT.HIERARCHY</v>
       </c>
       <c r="C8" t="b">
@@ -59547,7 +59568,7 @@
         <v>782</v>
       </c>
       <c r="B9" t="str">
-        <f>ApplicationDef!$AJ$2</f>
+        <f>ApplicationDef!$AL$2</f>
         <v>PRODUCT.HIERARCHY</v>
       </c>
       <c r="C9" t="b">
@@ -59562,7 +59583,7 @@
         <v>784</v>
       </c>
       <c r="B10" t="str">
-        <f>ApplicationDef!$AF$2</f>
+        <f>ApplicationDef!$AH$2</f>
         <v>TIME</v>
       </c>
       <c r="C10" t="b">
@@ -59577,7 +59598,7 @@
         <v>786</v>
       </c>
       <c r="B11" t="str">
-        <f>ApplicationDef!$AF$2</f>
+        <f>ApplicationDef!$AH$2</f>
         <v>TIME</v>
       </c>
       <c r="C11" t="b">
@@ -60055,7 +60076,7 @@
         <v>826</v>
       </c>
       <c r="D4" t="str">
-        <f>ApplicationDef!$AF$2</f>
+        <f>ApplicationDef!$AH$2</f>
         <v>TIME</v>
       </c>
       <c r="E4" t="b">
@@ -60067,7 +60088,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="D5" t="str">
-        <f>ApplicationDef!$AI$2</f>
+        <f>ApplicationDef!$AK$2</f>
         <v>YEAR</v>
       </c>
     </row>
@@ -60102,7 +60123,7 @@
         <v>831</v>
       </c>
       <c r="D7" t="str">
-        <f>ApplicationDef!$AF$2</f>
+        <f>ApplicationDef!$AH$2</f>
         <v>TIME</v>
       </c>
       <c r="E7" t="b">
@@ -60114,7 +60135,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="D8" t="str">
-        <f>ApplicationDef!$AI$2</f>
+        <f>ApplicationDef!$AK$2</f>
         <v>YEAR</v>
       </c>
     </row>
@@ -61441,7 +61462,7 @@
         <v>CMWP</v>
       </c>
       <c r="F37" t="str">
-        <f>ApplicationDef!$AF$2</f>
+        <f>ApplicationDef!$AH$2</f>
         <v>TIME</v>
       </c>
       <c r="G37" t="s">
@@ -61464,7 +61485,7 @@
         <v>MWP</v>
       </c>
       <c r="F38" t="str">
-        <f>ApplicationDef!$AF$2</f>
+        <f>ApplicationDef!$AH$2</f>
         <v>TIME</v>
       </c>
       <c r="G38" t="s">
@@ -61487,7 +61508,7 @@
         <v>MP</v>
       </c>
       <c r="F39" t="str">
-        <f>ApplicationDef!$AF$2</f>
+        <f>ApplicationDef!$AH$2</f>
         <v>TIME</v>
       </c>
       <c r="G39" t="s">
@@ -61510,7 +61531,7 @@
         <v>LYR</v>
       </c>
       <c r="F40" t="str">
-        <f>ApplicationDef!$AF$2</f>
+        <f>ApplicationDef!$AH$2</f>
         <v>TIME</v>
       </c>
       <c r="G40" t="s">
@@ -61533,7 +61554,7 @@
         <v>MFP</v>
       </c>
       <c r="F41" t="str">
-        <f>ApplicationDef!$AF$2</f>
+        <f>ApplicationDef!$AH$2</f>
         <v>TIME</v>
       </c>
       <c r="G41" t="s">
@@ -61556,7 +61577,7 @@
         <v>MWP</v>
       </c>
       <c r="F42" t="str">
-        <f>ApplicationDef!$AJ$2</f>
+        <f>ApplicationDef!$AL$2</f>
         <v>PRODUCT.HIERARCHY</v>
       </c>
       <c r="G42" t="s">
@@ -61579,7 +61600,7 @@
         <v>MF</v>
       </c>
       <c r="F43" t="str">
-        <f>ApplicationDef!$AJ$2</f>
+        <f>ApplicationDef!$AL$2</f>
         <v>PRODUCT.HIERARCHY</v>
       </c>
       <c r="G43" t="s">
@@ -62264,7 +62285,7 @@
         <v>CMWF</v>
       </c>
       <c r="F78" t="str">
-        <f>ApplicationDef!$AF$2</f>
+        <f>ApplicationDef!$AH$2</f>
         <v>TIME</v>
       </c>
       <c r="G78" t="s">
@@ -62287,7 +62308,7 @@
         <v>MWF</v>
       </c>
       <c r="F79" t="str">
-        <f>ApplicationDef!$AF$2</f>
+        <f>ApplicationDef!$AH$2</f>
         <v>TIME</v>
       </c>
       <c r="G79" t="s">
@@ -62310,7 +62331,7 @@
         <v>MF</v>
       </c>
       <c r="F80" t="str">
-        <f>ApplicationDef!$AF$2</f>
+        <f>ApplicationDef!$AH$2</f>
         <v>TIME</v>
       </c>
       <c r="G80" t="s">
@@ -62333,7 +62354,7 @@
         <v>MWF</v>
       </c>
       <c r="F81" t="str">
-        <f>ApplicationDef!$AJ$2</f>
+        <f>ApplicationDef!$AL$2</f>
         <v>PRODUCT.HIERARCHY</v>
       </c>
       <c r="G81" t="s">
@@ -62356,7 +62377,7 @@
         <v>MF</v>
       </c>
       <c r="F82" t="str">
-        <f>ApplicationDef!$AJ$2</f>
+        <f>ApplicationDef!$AL$2</f>
         <v>PRODUCT.HIERARCHY</v>
       </c>
       <c r="G82" t="s">
@@ -63246,7 +63267,7 @@
         <v>303</v>
       </c>
       <c r="B2" t="str">
-        <f>ApplicationDef!$AF$2</f>
+        <f>ApplicationDef!$AH$2</f>
         <v>TIME</v>
       </c>
       <c r="C2" t="s">
@@ -63265,7 +63286,7 @@
         <v>305</v>
       </c>
       <c r="B3" t="str">
-        <f>ApplicationDef!$AF$2</f>
+        <f>ApplicationDef!$AH$2</f>
         <v>TIME</v>
       </c>
       <c r="C3" t="s">

</xml_diff>